<commit_message>
Tópicos a serem explorados
</commit_message>
<xml_diff>
--- a/xlsx/painelcovid2_tabela_total_v1.xlsx
+++ b/xlsx/painelcovid2_tabela_total_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\OneDrive\Documentos\Unesp\Visu - Danilo\trabVisualizacaoInf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECAE6AF-EC1D-4391-BC08-021DDC6B29C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50624D9E-F893-46B3-A8FC-B1A959474058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C5W" sheetId="1" r:id="rId1"/>
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2101,7 +2101,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4058,6 +4060,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
@@ -4067,11 +4074,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="A16:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4082,7 +4084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6921,6 +6925,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="U3:Z3"/>
+    <mergeCell ref="AA3:AF3"/>
+    <mergeCell ref="AG3:AL3"/>
+    <mergeCell ref="AM3:AR3"/>
+    <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="I3:N3"/>
@@ -6930,11 +6939,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="U3:Z3"/>
-    <mergeCell ref="AA3:AF3"/>
-    <mergeCell ref="AG3:AL3"/>
-    <mergeCell ref="AM3:AR3"/>
-    <mergeCell ref="A16:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6945,7 +6949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9406,6 +9412,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:F3"/>
@@ -9416,12 +9428,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AE3:AH3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9432,7 +9438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9962,7 +9970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11919,6 +11929,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
@@ -11928,11 +11943,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="A16:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11943,7 +11953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12409,7 +12421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13003,7 +13017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13533,7 +13549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15994,6 +16012,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:F3"/>
@@ -16004,12 +16028,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AE3:AH3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16020,7 +16038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AU25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18985,6 +19005,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AM3:AP3"/>
+    <mergeCell ref="AQ3:AT3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:F3"/>
@@ -18995,14 +19023,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AM3:AP3"/>
-    <mergeCell ref="AQ3:AT3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AE3:AH3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -19013,7 +19033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -19982,7 +20004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -20951,7 +20975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21417,7 +21443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21883,7 +21911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22580,6 +22610,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:C4"/>
@@ -22590,11 +22625,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -22605,7 +22635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23135,7 +23167,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23665,7 +23699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24507,7 +24543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -25393,6 +25431,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C3:C4"/>
@@ -25403,14 +25449,6 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -25421,7 +25459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26390,7 +26430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26856,7 +26898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28078,7 +28122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28794,7 +28840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29324,7 +29372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29918,7 +29968,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31140,7 +31192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31858,7 +31912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -32452,7 +32508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34180,7 +34238,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34646,7 +34706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35615,7 +35677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -36837,7 +36901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -37493,7 +37559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -37895,7 +37963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -38611,7 +38681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -39077,7 +39149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>